<commit_message>
Fix issue #344 8b74eef7e5c0dc0449a502579f324ce1e4eab437
</commit_message>
<xml_diff>
--- a/344-spécifications-techniques---séparation-des-modèles-sdo-et-esms/ig/CodeSystem-input-task-sdo-codesystem.xlsx
+++ b/344-spécifications-techniques---séparation-des-modèles-sdo-et-esms/ig/CodeSystem-input-task-sdo-codesystem.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-04T08:10:47+00:00</t>
+    <t>2025-12-04T16:15:01+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,7 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Code System pour la définition des éléments spécifiques de input dans ressource SDOTask</t>
+    <t>Code System pour la définition des éléments spécifiques de input dans ressource ESMSTask</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>